<commit_message>
Realicé pruebas para llenar formatos de excel
</commit_message>
<xml_diff>
--- a/Plantillas/Autorizaciones.xlsx
+++ b/Plantillas/Autorizaciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tipo de Solicitud </t>
-  </si>
-  <si>
-    <t>COM-016</t>
   </si>
   <si>
     <t>Autorización No.:</t>
@@ -573,21 +570,102 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,87 +698,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +736,7 @@
         <xdr:cNvPr id="2" name="Rectángulo 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE33A7F-43E6-4516-8071-3E198058B525}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBE33A7F-43E6-4516-8071-3E198058B525}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -801,7 +798,7 @@
         <xdr:cNvPr id="3" name="Rectángulo 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972BB1A4-66EA-4098-B18B-6AD5563AD25F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{972BB1A4-66EA-4098-B18B-6AD5563AD25F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -863,7 +860,7 @@
         <xdr:cNvPr id="4" name="Rectángulo 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AA7BD9A-3751-419C-AD33-90DC2BB7898E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2AA7BD9A-3751-419C-AD33-90DC2BB7898E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -925,7 +922,7 @@
         <xdr:cNvPr id="5" name="Rectángulo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5824D9B6-C231-432D-B746-9D1221C5B2FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5824D9B6-C231-432D-B746-9D1221C5B2FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -982,7 +979,7 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC46AD3-E9ED-47EA-AED6-54B4677993D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FC46AD3-E9ED-47EA-AED6-54B4677993D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1006,90 +1003,6 @@
         <a:xfrm>
           <a:off x="278423" y="29308"/>
           <a:ext cx="585093" cy="710658"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>71767</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>65879</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="229471" cy="281102"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19CAFAE9-A145-324F-E6F2-0A1997D231DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6139192" y="1694654"/>
-          <a:ext cx="229471" cy="281102"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>61231</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1006340" cy="341539"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62542E3F-B8F5-4573-8960-13CCD268FAF2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="880382" y="6576331"/>
-          <a:ext cx="1006340" cy="341539"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1366,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:H17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,57 +1296,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="76"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="36">
         <v>45505</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,13 +1365,11 @@
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
-      <c r="F6" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="78"/>
-      <c r="H6" s="29" t="s">
+      <c r="F6" s="47" t="s">
         <v>21</v>
       </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
@@ -1471,16 +1382,16 @@
       <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
@@ -1493,10 +1404,10 @@
       <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="80"/>
+      <c r="B10" s="49"/>
       <c r="D10" s="25" t="s">
         <v>18</v>
       </c>
@@ -1511,50 +1422,50 @@
     </row>
     <row r="11" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="66"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="1"/>
       <c r="F12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="1"/>
       <c r="F13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="70"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
     </row>
@@ -1568,15 +1479,15 @@
       <c r="C16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65" t="s">
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="65"/>
+      <c r="H16" s="60"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -1584,13 +1495,13 @@
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="41"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -1598,11 +1509,11 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="41"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="51"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -1610,11 +1521,11 @@
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="41"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
@@ -1622,11 +1533,11 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="41"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -1634,11 +1545,11 @@
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="41"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
@@ -1646,11 +1557,11 @@
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="41"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
@@ -1658,11 +1569,11 @@
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="41"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
@@ -1670,9 +1581,9 @@
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="51"/>
       <c r="G24" s="17"/>
       <c r="H24" s="16"/>
     </row>
@@ -1682,9 +1593,9 @@
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="51"/>
       <c r="G25" s="17"/>
       <c r="H25" s="16"/>
     </row>
@@ -1694,11 +1605,11 @@
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="41"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
@@ -1706,11 +1617,11 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="41"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
@@ -1718,9 +1629,9 @@
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="51"/>
       <c r="G28" s="12"/>
       <c r="H28" s="11"/>
     </row>
@@ -1730,69 +1641,69 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="41"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="77"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="58"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="66"/>
     </row>
     <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
     </row>
     <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -1805,17 +1716,17 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="G36" s="60" t="s">
+      <c r="G36" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="60"/>
+      <c r="H36" s="68"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
@@ -1823,39 +1734,39 @@
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
+      <c r="A39" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
       <c r="D39" s="1"/>
-      <c r="G39" s="55" t="s">
+      <c r="G39" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="55"/>
+      <c r="H39" s="63"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
+      <c r="B40" s="79"/>
+      <c r="C40" s="79"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="53"/>
+      <c r="H40" s="80"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -1866,8 +1777,8 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="1"/>
     </row>
   </sheetData>
@@ -1880,13 +1791,35 @@
     <protectedRange sqref="C19:C20" name="Rango1_6_1_1"/>
   </protectedRanges>
   <mergeCells count="52">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G37:H38"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A33:H34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
@@ -1903,35 +1836,13 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:H34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G37:H38"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se llenan los dos formatos correctamente
</commit_message>
<xml_diff>
--- a/Plantillas/Autorizaciones.xlsx
+++ b/Plantillas/Autorizaciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -526,16 +526,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,6 +566,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,48 +617,42 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -678,26 +686,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,258 +741,10 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>58969</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>72684</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>286399</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>305829</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectángulo 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBE33A7F-43E6-4516-8071-3E198058B525}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6126394" y="1701459"/>
-          <a:ext cx="227430" cy="109320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1048760</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>72684</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>37940</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>300114</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectángulo 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{972BB1A4-66EA-4098-B18B-6AD5563AD25F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3468110" y="1701459"/>
-          <a:ext cx="36930" cy="103605"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>627533</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>72684</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>211806</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>305829</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectángulo 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2AA7BD9A-3751-419C-AD33-90DC2BB7898E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4961408" y="1701459"/>
-          <a:ext cx="451048" cy="109320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>516401</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>45469</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>56910</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>278242</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectángulo 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5824D9B6-C231-432D-B746-9D1221C5B2FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1383176" y="1674244"/>
-          <a:ext cx="407284" cy="137523"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>278423</xdr:colOff>
+      <xdr:colOff>211187</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>29308</xdr:rowOff>
     </xdr:from>
@@ -1001,7 +776,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="278423" y="29308"/>
+          <a:off x="211187" y="29308"/>
           <a:ext cx="585093" cy="710658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1280,15 +1055,15 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B30" sqref="B30:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
@@ -1296,176 +1071,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="37" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="33">
         <v>45505</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="31" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="30"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="47" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="29"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-    </row>
-    <row r="9" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="H9" s="36"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="D10" s="25" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="23" t="s">
+      <c r="D10" s="40"/>
+      <c r="E10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="1"/>
       <c r="F12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="1"/>
       <c r="F13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
     </row>
@@ -1479,15 +1253,15 @@
       <c r="C16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60" t="s">
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="60"/>
+      <c r="H16" s="61"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -1495,13 +1269,11 @@
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="50" t="s">
-        <v>6</v>
-      </c>
+      <c r="D17" s="54"/>
       <c r="E17" s="55"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="56"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -1509,11 +1281,11 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="55"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="51"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="56"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -1521,11 +1293,11 @@
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
-      <c r="D19" s="50"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="55"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="51"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="56"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
@@ -1533,11 +1305,11 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="55"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -1545,11 +1317,11 @@
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="55"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="56"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
@@ -1557,11 +1329,11 @@
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="55"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
@@ -1569,11 +1341,11 @@
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="50"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="55"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="51"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="56"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
@@ -1581,9 +1353,9 @@
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="50"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="55"/>
-      <c r="F24" s="51"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="17"/>
       <c r="H24" s="16"/>
     </row>
@@ -1593,9 +1365,9 @@
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="50"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="55"/>
-      <c r="F25" s="51"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="17"/>
       <c r="H25" s="16"/>
     </row>
@@ -1605,11 +1377,11 @@
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="50"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="55"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="51"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
@@ -1617,11 +1389,11 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="50"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="55"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="56"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
@@ -1629,9 +1401,9 @@
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="50"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="55"/>
-      <c r="F28" s="51"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="12"/>
       <c r="H28" s="11"/>
     </row>
@@ -1641,69 +1413,69 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="51"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="56"/>
     </row>
     <row r="30" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
       <c r="H31" s="77"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="66"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="68"/>
     </row>
     <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
     </row>
     <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -1716,17 +1488,17 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="G36" s="68" t="s">
+      <c r="G36" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="68"/>
+      <c r="H36" s="70"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
@@ -1734,39 +1506,39 @@
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="62" t="s">
+      <c r="A39" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
+      <c r="B39" s="79"/>
+      <c r="C39" s="79"/>
       <c r="D39" s="1"/>
-      <c r="G39" s="63" t="s">
+      <c r="G39" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="63"/>
+      <c r="H39" s="65"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="78" t="s">
+      <c r="A40" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="79"/>
-      <c r="C40" s="79"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="80"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="80" t="s">
+      <c r="G40" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="80"/>
+      <c r="H40" s="78"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -1777,8 +1549,8 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="1"/>
     </row>
   </sheetData>
@@ -1790,8 +1562,10 @@
     <protectedRange sqref="B19:B20" name="Rango1_5_1_1"/>
     <protectedRange sqref="C19:C20" name="Rango1_6_1_1"/>
   </protectedRanges>
-  <mergeCells count="52">
-    <mergeCell ref="G22:H22"/>
+  <mergeCells count="49">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="G37:H38"/>
@@ -1800,16 +1574,13 @@
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A40:C40"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A39:C39"/>
     <mergeCell ref="G39:H39"/>
-    <mergeCell ref="A32:H32"/>
     <mergeCell ref="A33:H34"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="D24:F24"/>
@@ -1820,15 +1591,12 @@
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D16:F16"/>
@@ -1836,13 +1604,14 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:H3"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Relacion de contratos con Auto y Sol
</commit_message>
<xml_diff>
--- a/Plantillas/Autorizaciones.xlsx
+++ b/Plantillas/Autorizaciones.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sistema_SPagos\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gestor-Autorizaciones y Pagos\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A071C15-E8F7-4CA9-AC46-65C2B939D2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="-28920" yWindow="-3900" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSPA Canrig" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -165,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
@@ -465,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,175 +520,207 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -686,41 +730,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,7 +761,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>211187</xdr:colOff>
+      <xdr:colOff>558569</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>29308</xdr:rowOff>
     </xdr:from>
@@ -754,7 +771,7 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FC46AD3-E9ED-47EA-AED6-54B4677993D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC46AD3-E9ED-47EA-AED6-54B4677993D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -776,7 +793,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="211187" y="29308"/>
+          <a:off x="558569" y="29308"/>
           <a:ext cx="585093" cy="710658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1051,217 +1068,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="34" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="31">
         <v>45505</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="27"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="51" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="26"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="H9" s="36"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="38" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="37" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
     </row>
     <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="64" t="s">
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61" t="s">
+      <c r="E16" s="62"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="61"/>
+      <c r="H16" s="64"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -1269,11 +1286,11 @@
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="66"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -1281,35 +1298,35 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="66"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>3</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="56"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="66"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>4</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="56"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="66"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -1317,11 +1334,11 @@
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="66"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
@@ -1329,11 +1346,11 @@
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="66"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
@@ -1341,11 +1358,11 @@
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="66"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
@@ -1353,11 +1370,11 @@
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="16"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="66"/>
     </row>
     <row r="25" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
@@ -1365,11 +1382,11 @@
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="16"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="90"/>
     </row>
     <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
@@ -1377,11 +1394,11 @@
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="66"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
@@ -1389,11 +1406,11 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="59"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
@@ -1401,9 +1418,9 @@
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="59"/>
       <c r="G28" s="12"/>
       <c r="H28" s="11"/>
     </row>
@@ -1413,69 +1430,69 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="56"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="59"/>
     </row>
     <row r="30" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="86" t="s">
+      <c r="A30" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="83"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="77"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="75"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="68"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="78"/>
     </row>
     <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
     </row>
     <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
+      <c r="A34" s="71"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -1488,17 +1505,17 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="G36" s="70" t="s">
+      <c r="G36" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="70"/>
+      <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
@@ -1506,39 +1523,38 @@
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
+      <c r="H38" s="45"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="40" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="1"/>
-      <c r="G39" s="65" t="s">
+      <c r="G39" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="65"/>
+      <c r="H39" s="70"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="82" t="s">
+      <c r="A40" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="80"/>
       <c r="C40" s="80"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="78" t="s">
+      <c r="G40" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="78"/>
+      <c r="H40" s="88"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -1549,8 +1565,8 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="1"/>
     </row>
   </sheetData>
@@ -1562,22 +1578,21 @@
     <protectedRange sqref="B19:B20" name="Rango1_5_1_1"/>
     <protectedRange sqref="C19:C20" name="Rango1_6_1_1"/>
   </protectedRanges>
-  <mergeCells count="49">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
+  <mergeCells count="50">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G37:H38"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G39:H39"/>
@@ -1592,6 +1607,8 @@
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="D18:F18"/>

</xml_diff>

<commit_message>
Adicion del modulo de costos por contrato
</commit_message>
<xml_diff>
--- a/Plantillas/Autorizaciones.xlsx
+++ b/Plantillas/Autorizaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gestor-Autorizaciones y Pagos\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A071C15-E8F7-4CA9-AC46-65C2B939D2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D009439-8BE7-46BD-A7F0-468B60B751AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3900" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSPA Canrig" sheetId="1" r:id="rId1"/>
@@ -477,12 +477,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -584,26 +581,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,65 +673,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -730,14 +709,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,486 +1085,1306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="53" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="43" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>45505</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="25"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="54" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="24"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="H9" s="33"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="34" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
     </row>
     <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="69" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="69"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64" t="s">
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="64"/>
+      <c r="H16" s="68"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>1</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="66"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="70"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>2</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="70"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>3</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="66"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="70"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>4</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="70"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>5</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="66"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="70"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="70"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>7</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="70"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>8</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="66"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="70"/>
     </row>
     <row r="25" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>9</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="90"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="70"/>
     </row>
     <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="13">
         <v>10</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="66"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="70"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>10</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="59"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="63"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>11</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="11"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="8.4499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>12</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="59"/>
-    </row>
-    <row r="30" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="63"/>
+    </row>
+    <row r="30" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="83"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="B30" s="84"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="86"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="75"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="83"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="78"/>
-    </row>
-    <row r="33" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71" t="s">
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="88"/>
+      <c r="H32" s="89"/>
+    </row>
+    <row r="33" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+    </row>
+    <row r="35" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72" t="s">
+      <c r="A36" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="G36" s="72" t="s">
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="G36" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="72"/>
+      <c r="H36" s="49"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="H38" s="45"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="H38" s="39"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="79"/>
-      <c r="C39" s="79"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
       <c r="D39" s="1"/>
-      <c r="G39" s="70" t="s">
+      <c r="G39" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="70"/>
+      <c r="H39" s="77"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="80"/>
-      <c r="C40" s="80"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="88" t="s">
+      <c r="G40" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="88"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="1"/>
+      <c r="H40" s="40"/>
+    </row>
+    <row r="41" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="45"/>
+      <c r="C54" s="45"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="45"/>
+      <c r="C57" s="45"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="45"/>
+      <c r="C61" s="45"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="45"/>
+      <c r="C63" s="45"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="45"/>
+      <c r="C64" s="45"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="45"/>
+      <c r="C67" s="45"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="45"/>
+      <c r="C68" s="45"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="45"/>
+      <c r="C70" s="45"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="45"/>
+      <c r="C71" s="45"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="45"/>
+      <c r="C73" s="45"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="45"/>
+      <c r="C74" s="45"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="45"/>
+      <c r="C75" s="45"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="45"/>
+      <c r="C76" s="45"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="45"/>
+      <c r="C77" s="45"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="45"/>
+      <c r="C79" s="45"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="45"/>
+      <c r="C80" s="45"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="45"/>
+      <c r="C81" s="45"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="45"/>
+      <c r="C82" s="45"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="45"/>
+      <c r="C83" s="45"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="45"/>
+      <c r="C84" s="45"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="45"/>
+      <c r="C85" s="45"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="45"/>
+      <c r="C86" s="45"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="45"/>
+      <c r="C87" s="45"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="45"/>
+      <c r="C88" s="45"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="45"/>
+      <c r="C89" s="45"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="45"/>
+      <c r="C90" s="45"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="45"/>
+      <c r="C91" s="45"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="45"/>
+      <c r="C92" s="45"/>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="45"/>
+      <c r="C93" s="45"/>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="45"/>
+      <c r="C94" s="45"/>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="45"/>
+      <c r="C95" s="45"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="45"/>
+      <c r="C96" s="45"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="45"/>
+      <c r="C97" s="45"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="45"/>
+      <c r="C98" s="45"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="45"/>
+      <c r="C99" s="45"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="45"/>
+      <c r="C100" s="45"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="45"/>
+      <c r="C101" s="45"/>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="45"/>
+      <c r="C102" s="45"/>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="45"/>
+      <c r="C103" s="45"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="45"/>
+      <c r="C104" s="45"/>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="45"/>
+      <c r="C105" s="45"/>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="45"/>
+      <c r="C106" s="45"/>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="45"/>
+      <c r="C107" s="45"/>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="45"/>
+      <c r="C108" s="45"/>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="45"/>
+      <c r="C109" s="45"/>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="45"/>
+      <c r="C110" s="45"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="45"/>
+      <c r="C111" s="45"/>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="45"/>
+      <c r="C112" s="45"/>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="45"/>
+      <c r="C113" s="45"/>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="45"/>
+      <c r="C114" s="45"/>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" s="45"/>
+      <c r="C115" s="45"/>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="45"/>
+      <c r="C116" s="45"/>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="45"/>
+      <c r="C117" s="45"/>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="45"/>
+      <c r="C118" s="45"/>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="45"/>
+      <c r="C119" s="45"/>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="45"/>
+      <c r="C120" s="45"/>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="45"/>
+      <c r="C121" s="45"/>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="45"/>
+      <c r="C122" s="45"/>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="45"/>
+      <c r="C123" s="45"/>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="45"/>
+      <c r="C124" s="45"/>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="45"/>
+      <c r="C125" s="45"/>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="45"/>
+      <c r="C126" s="45"/>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="45"/>
+      <c r="C127" s="45"/>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="45"/>
+      <c r="C128" s="45"/>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="45"/>
+      <c r="C129" s="45"/>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="45"/>
+      <c r="C130" s="45"/>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" s="45"/>
+      <c r="C131" s="45"/>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="45"/>
+      <c r="C132" s="45"/>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="45"/>
+      <c r="C133" s="45"/>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="45"/>
+      <c r="C134" s="45"/>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="45"/>
+      <c r="C135" s="45"/>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" s="45"/>
+      <c r="C136" s="45"/>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" s="45"/>
+      <c r="C137" s="45"/>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" s="45"/>
+      <c r="C138" s="45"/>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" s="45"/>
+      <c r="C139" s="45"/>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" s="45"/>
+      <c r="C140" s="45"/>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" s="45"/>
+      <c r="C141" s="45"/>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" s="45"/>
+      <c r="C142" s="45"/>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" s="45"/>
+      <c r="C143" s="45"/>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" s="45"/>
+      <c r="C144" s="45"/>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="45"/>
+      <c r="C145" s="45"/>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="45"/>
+      <c r="C146" s="45"/>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="45"/>
+      <c r="C147" s="45"/>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="45"/>
+      <c r="C148" s="45"/>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" s="45"/>
+      <c r="C149" s="45"/>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="45"/>
+      <c r="C150" s="45"/>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="45"/>
+      <c r="C151" s="45"/>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="45"/>
+      <c r="C152" s="45"/>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="45"/>
+      <c r="C153" s="45"/>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="45"/>
+      <c r="C154" s="45"/>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="45"/>
+      <c r="C155" s="45"/>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="45"/>
+      <c r="C156" s="45"/>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" s="45"/>
+      <c r="C157" s="45"/>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="45"/>
+      <c r="C158" s="45"/>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B159" s="45"/>
+      <c r="C159" s="45"/>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B160" s="45"/>
+      <c r="C160" s="45"/>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" s="45"/>
+      <c r="C161" s="45"/>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="45"/>
+      <c r="C162" s="45"/>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" s="45"/>
+      <c r="C163" s="45"/>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" s="45"/>
+      <c r="C164" s="45"/>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" s="45"/>
+      <c r="C165" s="45"/>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" s="45"/>
+      <c r="C166" s="45"/>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="45"/>
+      <c r="C167" s="45"/>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" s="45"/>
+      <c r="C168" s="45"/>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B169" s="45"/>
+      <c r="C169" s="45"/>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="45"/>
+      <c r="C170" s="45"/>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171" s="45"/>
+      <c r="C171" s="45"/>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" s="45"/>
+      <c r="C172" s="45"/>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="45"/>
+      <c r="C173" s="45"/>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" s="45"/>
+      <c r="C174" s="45"/>
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B175" s="45"/>
+      <c r="C175" s="45"/>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" s="45"/>
+      <c r="C176" s="45"/>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" s="45"/>
+      <c r="C177" s="45"/>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" s="45"/>
+      <c r="C178" s="45"/>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="45"/>
+      <c r="C179" s="45"/>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" s="45"/>
+      <c r="C180" s="45"/>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" s="45"/>
+      <c r="C181" s="45"/>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" s="45"/>
+      <c r="C182" s="45"/>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B183" s="45"/>
+      <c r="C183" s="45"/>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B184" s="45"/>
+      <c r="C184" s="45"/>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" s="45"/>
+      <c r="C185" s="45"/>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" s="45"/>
+      <c r="C186" s="45"/>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" s="45"/>
+      <c r="C187" s="45"/>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B188" s="45"/>
+      <c r="C188" s="45"/>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="45"/>
+      <c r="C189" s="45"/>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B190" s="45"/>
+      <c r="C190" s="45"/>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" s="45"/>
+      <c r="C191" s="45"/>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="45"/>
+      <c r="C192" s="45"/>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="45"/>
+      <c r="C193" s="45"/>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="45"/>
+      <c r="C194" s="45"/>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="45"/>
+      <c r="C195" s="45"/>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="45"/>
+      <c r="C196" s="45"/>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="45"/>
+      <c r="C197" s="45"/>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="45"/>
+      <c r="C198" s="45"/>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="45"/>
+      <c r="C199" s="45"/>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="45"/>
+      <c r="C200" s="45"/>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="45"/>
+      <c r="C201" s="45"/>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="45"/>
+      <c r="C202" s="45"/>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="45"/>
+      <c r="C203" s="45"/>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="45"/>
+      <c r="C204" s="45"/>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="45"/>
+      <c r="C205" s="45"/>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B206" s="45"/>
+      <c r="C206" s="45"/>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" s="45"/>
+      <c r="C207" s="45"/>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="45"/>
+      <c r="C208" s="45"/>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" s="45"/>
+      <c r="C209" s="45"/>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="45"/>
+      <c r="C210" s="45"/>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="45"/>
+      <c r="C211" s="45"/>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="45"/>
+      <c r="C212" s="45"/>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="45"/>
+      <c r="C213" s="45"/>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="45"/>
+      <c r="C214" s="45"/>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="45"/>
+      <c r="C215" s="45"/>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="45"/>
+      <c r="C216" s="45"/>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="45"/>
+      <c r="C217" s="45"/>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" s="45"/>
+      <c r="C218" s="45"/>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="45"/>
+      <c r="C219" s="45"/>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="45"/>
+      <c r="C220" s="45"/>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B221" s="45"/>
+      <c r="C221" s="45"/>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B222" s="45"/>
+      <c r="C222" s="45"/>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="45"/>
+      <c r="C223" s="45"/>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B224" s="45"/>
+      <c r="C224" s="45"/>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B225" s="45"/>
+      <c r="C225" s="45"/>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B226" s="45"/>
+      <c r="C226" s="45"/>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227" s="45"/>
+      <c r="C227" s="45"/>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B228" s="45"/>
+      <c r="C228" s="45"/>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B229" s="45"/>
+      <c r="C229" s="45"/>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B230" s="45"/>
+      <c r="C230" s="45"/>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B231" s="45"/>
+      <c r="C231" s="45"/>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B232" s="45"/>
+      <c r="C232" s="45"/>
+    </row>
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B233" s="45"/>
+      <c r="C233" s="45"/>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B234" s="45"/>
+      <c r="C234" s="45"/>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B235" s="45"/>
+      <c r="C235" s="45"/>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B236" s="45"/>
+      <c r="C236" s="45"/>
+    </row>
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B237" s="45"/>
+      <c r="C237" s="45"/>
+    </row>
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B238" s="45"/>
+      <c r="C238" s="45"/>
+    </row>
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B239" s="45"/>
+      <c r="C239" s="45"/>
+    </row>
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B240" s="45"/>
+      <c r="C240" s="45"/>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B241" s="45"/>
+      <c r="C241" s="45"/>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B242" s="45"/>
+      <c r="C242" s="45"/>
+    </row>
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B243" s="45"/>
+      <c r="C243" s="45"/>
+    </row>
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B244" s="45"/>
+      <c r="C244" s="45"/>
+    </row>
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B245" s="45"/>
+      <c r="C245" s="45"/>
+    </row>
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B246" s="45"/>
+      <c r="C246" s="45"/>
+    </row>
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B247" s="45"/>
+      <c r="C247" s="45"/>
+    </row>
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B248" s="45"/>
+      <c r="C248" s="45"/>
+    </row>
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B249" s="45"/>
+      <c r="C249" s="45"/>
+    </row>
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B250" s="45"/>
+      <c r="C250" s="45"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -1578,42 +2395,36 @@
     <protectedRange sqref="B19:B20" name="Rango1_5_1_1"/>
     <protectedRange sqref="C19:C20" name="Rango1_6_1_1"/>
   </protectedRanges>
-  <mergeCells count="50">
+  <mergeCells count="48">
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="G23:H23"/>
-    <mergeCell ref="D42:E42"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G40:H40"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="A33:H34"/>
-    <mergeCell ref="A36:C36"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D16:F16"/>
@@ -1623,12 +2434,16 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:H36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version con modificaciones y prueba de actualizador
</commit_message>
<xml_diff>
--- a/Plantillas/Autorizaciones.xlsx
+++ b/Plantillas/Autorizaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maestra Flor\Gestor-Autorizaciones y Pagos\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3EFBA6-6418-4C11-8CEC-DF5E1A420507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3830355-8A5F-478F-B37B-677D1FF080C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="3150" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSPA Canrig" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <r>
       <rPr>
@@ -173,13 +173,17 @@
   <si>
     <t xml:space="preserve">Nombre: </t>
   </si>
+  <si>
+    <t>Cotización:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -236,14 +240,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -293,6 +289,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -320,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -473,11 +477,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,231 +542,237 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,15 +1106,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="81" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37:H38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="95" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
@@ -1089,40 +1123,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="65" t="s">
+      <c r="A1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="37" t="s">
         <v>26</v>
       </c>
@@ -1158,10 +1192,10 @@
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="75"/>
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1175,16 +1209,16 @@
       <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
@@ -1217,47 +1251,47 @@
       <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="1"/>
       <c r="F12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
     </row>
     <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="1"/>
       <c r="F13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
     </row>
     <row r="14" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="58" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
     </row>
@@ -1271,15 +1305,15 @@
       <c r="C16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51" t="s">
+      <c r="E16" s="82"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="51"/>
+      <c r="H16" s="84"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
@@ -1287,11 +1321,11 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="55"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -1299,11 +1333,11 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="53"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="55"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -1311,11 +1345,11 @@
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="53"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="55"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -1323,11 +1357,11 @@
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="53"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -1335,11 +1369,11 @@
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="53"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="55"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -1347,11 +1381,11 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="53"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="55"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -1359,11 +1393,11 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="53"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="55"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -1371,11 +1405,11 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="53"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="55"/>
     </row>
     <row r="25" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -1383,11 +1417,11 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="53"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
@@ -1395,11 +1429,11 @@
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="53"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="55"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
@@ -1407,11 +1441,11 @@
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="12"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="46"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="53"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
@@ -1419,9 +1453,9 @@
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="53"/>
       <c r="G28" s="11"/>
       <c r="H28" s="10"/>
     </row>
@@ -1431,69 +1465,71 @@
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="46"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="53"/>
     </row>
     <row r="30" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="75"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="81"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="78"/>
+      <c r="A31" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="62"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="65"/>
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="45"/>
     </row>
     <row r="34" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
     </row>
     <row r="35" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
@@ -1506,17 +1542,17 @@
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="88"/>
-      <c r="C36" s="88"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="G36" s="88" t="s">
+      <c r="G36" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="88"/>
+      <c r="H36" s="46"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -1524,872 +1560,872 @@
       <c r="C37" s="4"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
       <c r="D39" s="1"/>
-      <c r="G39" s="87" t="s">
+      <c r="G39" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="87"/>
+      <c r="H39" s="90"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="88"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="38" t="s">
+      <c r="G40" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="38"/>
+      <c r="H40" s="91"/>
     </row>
     <row r="41" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="41"/>
-      <c r="C57" s="41"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="41"/>
-      <c r="C62" s="41"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="41"/>
-      <c r="C64" s="41"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="41"/>
-      <c r="C65" s="41"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="41"/>
-      <c r="C66" s="41"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="41"/>
-      <c r="C70" s="41"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="41"/>
-      <c r="C71" s="41"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="41"/>
-      <c r="C74" s="41"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="41"/>
-      <c r="C75" s="41"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="41"/>
-      <c r="C76" s="41"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="41"/>
-      <c r="C77" s="41"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="41"/>
-      <c r="C78" s="41"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="41"/>
-      <c r="C79" s="41"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="41"/>
-      <c r="C80" s="41"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="41"/>
-      <c r="C81" s="41"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="41"/>
-      <c r="C82" s="41"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="41"/>
-      <c r="C83" s="41"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="41"/>
-      <c r="C84" s="41"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="41"/>
-      <c r="C85" s="41"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="41"/>
-      <c r="C86" s="41"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="41"/>
-      <c r="C87" s="41"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="41"/>
-      <c r="C88" s="41"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="41"/>
-      <c r="C89" s="41"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="41"/>
-      <c r="C90" s="41"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="41"/>
-      <c r="C91" s="41"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="41"/>
-      <c r="C92" s="41"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="41"/>
-      <c r="C93" s="41"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="41"/>
-      <c r="C94" s="41"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="41"/>
-      <c r="C95" s="41"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="41"/>
-      <c r="C96" s="41"/>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="41"/>
-      <c r="C97" s="41"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="41"/>
-      <c r="C98" s="41"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="41"/>
-      <c r="C99" s="41"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="41"/>
-      <c r="C100" s="41"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="41"/>
-      <c r="C101" s="41"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="41"/>
-      <c r="C102" s="41"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="41"/>
-      <c r="C103" s="41"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="41"/>
-      <c r="C104" s="41"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="41"/>
-      <c r="C105" s="41"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="41"/>
-      <c r="C106" s="41"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="41"/>
-      <c r="C107" s="41"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="41"/>
-      <c r="C108" s="41"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="41"/>
-      <c r="C109" s="41"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="41"/>
-      <c r="C110" s="41"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="41"/>
-      <c r="C111" s="41"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="41"/>
-      <c r="C112" s="41"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="41"/>
-      <c r="C113" s="41"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="41"/>
-      <c r="C114" s="41"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115" s="41"/>
-      <c r="C115" s="41"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="41"/>
-      <c r="C116" s="41"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="41"/>
-      <c r="C117" s="41"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="41"/>
-      <c r="C118" s="41"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="41"/>
-      <c r="C119" s="41"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="41"/>
-      <c r="C120" s="41"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="41"/>
-      <c r="C121" s="41"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="41"/>
-      <c r="C122" s="41"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="41"/>
-      <c r="C123" s="41"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="41"/>
-      <c r="C124" s="41"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="41"/>
-      <c r="C125" s="41"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B126" s="41"/>
-      <c r="C126" s="41"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B127" s="41"/>
-      <c r="C127" s="41"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="41"/>
-      <c r="C128" s="41"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="38"/>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129" s="41"/>
-      <c r="C129" s="41"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="38"/>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130" s="41"/>
-      <c r="C130" s="41"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="38"/>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131" s="41"/>
-      <c r="C131" s="41"/>
+      <c r="B131" s="38"/>
+      <c r="C131" s="38"/>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="41"/>
-      <c r="C132" s="41"/>
+      <c r="B132" s="38"/>
+      <c r="C132" s="38"/>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B133" s="41"/>
-      <c r="C133" s="41"/>
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="41"/>
-      <c r="C134" s="41"/>
+      <c r="B134" s="38"/>
+      <c r="C134" s="38"/>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="41"/>
-      <c r="C135" s="41"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="38"/>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="41"/>
-      <c r="C136" s="41"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="38"/>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="41"/>
-      <c r="C137" s="41"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="41"/>
-      <c r="C138" s="41"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="38"/>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="41"/>
-      <c r="C139" s="41"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="41"/>
-      <c r="C140" s="41"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="38"/>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="41"/>
-      <c r="C141" s="41"/>
+      <c r="B141" s="38"/>
+      <c r="C141" s="38"/>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="41"/>
-      <c r="C142" s="41"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="38"/>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="41"/>
-      <c r="C143" s="41"/>
+      <c r="B143" s="38"/>
+      <c r="C143" s="38"/>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="41"/>
-      <c r="C144" s="41"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="41"/>
-      <c r="C145" s="41"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="41"/>
-      <c r="C146" s="41"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="38"/>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" s="41"/>
-      <c r="C147" s="41"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="38"/>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="41"/>
-      <c r="C148" s="41"/>
+      <c r="B148" s="38"/>
+      <c r="C148" s="38"/>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B149" s="41"/>
-      <c r="C149" s="41"/>
+      <c r="B149" s="38"/>
+      <c r="C149" s="38"/>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="41"/>
-      <c r="C150" s="41"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="38"/>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="41"/>
-      <c r="C151" s="41"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="38"/>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B152" s="41"/>
-      <c r="C152" s="41"/>
+      <c r="B152" s="38"/>
+      <c r="C152" s="38"/>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="41"/>
-      <c r="C153" s="41"/>
+      <c r="B153" s="38"/>
+      <c r="C153" s="38"/>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B154" s="41"/>
-      <c r="C154" s="41"/>
+      <c r="B154" s="38"/>
+      <c r="C154" s="38"/>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B155" s="41"/>
-      <c r="C155" s="41"/>
+      <c r="B155" s="38"/>
+      <c r="C155" s="38"/>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B156" s="41"/>
-      <c r="C156" s="41"/>
+      <c r="B156" s="38"/>
+      <c r="C156" s="38"/>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B157" s="41"/>
-      <c r="C157" s="41"/>
+      <c r="B157" s="38"/>
+      <c r="C157" s="38"/>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B158" s="41"/>
-      <c r="C158" s="41"/>
+      <c r="B158" s="38"/>
+      <c r="C158" s="38"/>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B159" s="41"/>
-      <c r="C159" s="41"/>
+      <c r="B159" s="38"/>
+      <c r="C159" s="38"/>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B160" s="41"/>
-      <c r="C160" s="41"/>
+      <c r="B160" s="38"/>
+      <c r="C160" s="38"/>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B161" s="41"/>
-      <c r="C161" s="41"/>
+      <c r="B161" s="38"/>
+      <c r="C161" s="38"/>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162" s="41"/>
-      <c r="C162" s="41"/>
+      <c r="B162" s="38"/>
+      <c r="C162" s="38"/>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="41"/>
-      <c r="C163" s="41"/>
+      <c r="B163" s="38"/>
+      <c r="C163" s="38"/>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164" s="41"/>
-      <c r="C164" s="41"/>
+      <c r="B164" s="38"/>
+      <c r="C164" s="38"/>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B165" s="41"/>
-      <c r="C165" s="41"/>
+      <c r="B165" s="38"/>
+      <c r="C165" s="38"/>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B166" s="41"/>
-      <c r="C166" s="41"/>
+      <c r="B166" s="38"/>
+      <c r="C166" s="38"/>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B167" s="41"/>
-      <c r="C167" s="41"/>
+      <c r="B167" s="38"/>
+      <c r="C167" s="38"/>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B168" s="41"/>
-      <c r="C168" s="41"/>
+      <c r="B168" s="38"/>
+      <c r="C168" s="38"/>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B169" s="41"/>
-      <c r="C169" s="41"/>
+      <c r="B169" s="38"/>
+      <c r="C169" s="38"/>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B170" s="41"/>
-      <c r="C170" s="41"/>
+      <c r="B170" s="38"/>
+      <c r="C170" s="38"/>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B171" s="41"/>
-      <c r="C171" s="41"/>
+      <c r="B171" s="38"/>
+      <c r="C171" s="38"/>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B172" s="41"/>
-      <c r="C172" s="41"/>
+      <c r="B172" s="38"/>
+      <c r="C172" s="38"/>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B173" s="41"/>
-      <c r="C173" s="41"/>
+      <c r="B173" s="38"/>
+      <c r="C173" s="38"/>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B174" s="41"/>
-      <c r="C174" s="41"/>
+      <c r="B174" s="38"/>
+      <c r="C174" s="38"/>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B175" s="41"/>
-      <c r="C175" s="41"/>
+      <c r="B175" s="38"/>
+      <c r="C175" s="38"/>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B176" s="41"/>
-      <c r="C176" s="41"/>
+      <c r="B176" s="38"/>
+      <c r="C176" s="38"/>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" s="41"/>
-      <c r="C177" s="41"/>
+      <c r="B177" s="38"/>
+      <c r="C177" s="38"/>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" s="41"/>
-      <c r="C178" s="41"/>
+      <c r="B178" s="38"/>
+      <c r="C178" s="38"/>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B179" s="41"/>
-      <c r="C179" s="41"/>
+      <c r="B179" s="38"/>
+      <c r="C179" s="38"/>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B180" s="41"/>
-      <c r="C180" s="41"/>
+      <c r="B180" s="38"/>
+      <c r="C180" s="38"/>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" s="41"/>
-      <c r="C181" s="41"/>
+      <c r="B181" s="38"/>
+      <c r="C181" s="38"/>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B182" s="41"/>
-      <c r="C182" s="41"/>
+      <c r="B182" s="38"/>
+      <c r="C182" s="38"/>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B183" s="41"/>
-      <c r="C183" s="41"/>
+      <c r="B183" s="38"/>
+      <c r="C183" s="38"/>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B184" s="41"/>
-      <c r="C184" s="41"/>
+      <c r="B184" s="38"/>
+      <c r="C184" s="38"/>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B185" s="41"/>
-      <c r="C185" s="41"/>
+      <c r="B185" s="38"/>
+      <c r="C185" s="38"/>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B186" s="41"/>
-      <c r="C186" s="41"/>
+      <c r="B186" s="38"/>
+      <c r="C186" s="38"/>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B187" s="41"/>
-      <c r="C187" s="41"/>
+      <c r="B187" s="38"/>
+      <c r="C187" s="38"/>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B188" s="41"/>
-      <c r="C188" s="41"/>
+      <c r="B188" s="38"/>
+      <c r="C188" s="38"/>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B189" s="41"/>
-      <c r="C189" s="41"/>
+      <c r="B189" s="38"/>
+      <c r="C189" s="38"/>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B190" s="41"/>
-      <c r="C190" s="41"/>
+      <c r="B190" s="38"/>
+      <c r="C190" s="38"/>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B191" s="41"/>
-      <c r="C191" s="41"/>
+      <c r="B191" s="38"/>
+      <c r="C191" s="38"/>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B192" s="41"/>
-      <c r="C192" s="41"/>
+      <c r="B192" s="38"/>
+      <c r="C192" s="38"/>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="41"/>
-      <c r="C193" s="41"/>
+      <c r="B193" s="38"/>
+      <c r="C193" s="38"/>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B194" s="41"/>
-      <c r="C194" s="41"/>
+      <c r="B194" s="38"/>
+      <c r="C194" s="38"/>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B195" s="41"/>
-      <c r="C195" s="41"/>
+      <c r="B195" s="38"/>
+      <c r="C195" s="38"/>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" s="41"/>
-      <c r="C196" s="41"/>
+      <c r="B196" s="38"/>
+      <c r="C196" s="38"/>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="41"/>
-      <c r="C197" s="41"/>
+      <c r="B197" s="38"/>
+      <c r="C197" s="38"/>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B198" s="41"/>
-      <c r="C198" s="41"/>
+      <c r="B198" s="38"/>
+      <c r="C198" s="38"/>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B199" s="41"/>
-      <c r="C199" s="41"/>
+      <c r="B199" s="38"/>
+      <c r="C199" s="38"/>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="41"/>
-      <c r="C200" s="41"/>
+      <c r="B200" s="38"/>
+      <c r="C200" s="38"/>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="41"/>
-      <c r="C201" s="41"/>
+      <c r="B201" s="38"/>
+      <c r="C201" s="38"/>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B202" s="41"/>
-      <c r="C202" s="41"/>
+      <c r="B202" s="38"/>
+      <c r="C202" s="38"/>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" s="41"/>
-      <c r="C203" s="41"/>
+      <c r="B203" s="38"/>
+      <c r="C203" s="38"/>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B204" s="41"/>
-      <c r="C204" s="41"/>
+      <c r="B204" s="38"/>
+      <c r="C204" s="38"/>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B205" s="41"/>
-      <c r="C205" s="41"/>
+      <c r="B205" s="38"/>
+      <c r="C205" s="38"/>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B206" s="41"/>
-      <c r="C206" s="41"/>
+      <c r="B206" s="38"/>
+      <c r="C206" s="38"/>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="41"/>
-      <c r="C207" s="41"/>
+      <c r="B207" s="38"/>
+      <c r="C207" s="38"/>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B208" s="41"/>
-      <c r="C208" s="41"/>
+      <c r="B208" s="38"/>
+      <c r="C208" s="38"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" s="41"/>
-      <c r="C209" s="41"/>
+      <c r="B209" s="38"/>
+      <c r="C209" s="38"/>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B210" s="41"/>
-      <c r="C210" s="41"/>
+      <c r="B210" s="38"/>
+      <c r="C210" s="38"/>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" s="41"/>
-      <c r="C211" s="41"/>
+      <c r="B211" s="38"/>
+      <c r="C211" s="38"/>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B212" s="41"/>
-      <c r="C212" s="41"/>
+      <c r="B212" s="38"/>
+      <c r="C212" s="38"/>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="41"/>
-      <c r="C213" s="41"/>
+      <c r="B213" s="38"/>
+      <c r="C213" s="38"/>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="41"/>
-      <c r="C214" s="41"/>
+      <c r="B214" s="38"/>
+      <c r="C214" s="38"/>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="41"/>
-      <c r="C215" s="41"/>
+      <c r="B215" s="38"/>
+      <c r="C215" s="38"/>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B216" s="41"/>
-      <c r="C216" s="41"/>
+      <c r="B216" s="38"/>
+      <c r="C216" s="38"/>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" s="41"/>
-      <c r="C217" s="41"/>
+      <c r="B217" s="38"/>
+      <c r="C217" s="38"/>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B218" s="41"/>
-      <c r="C218" s="41"/>
+      <c r="B218" s="38"/>
+      <c r="C218" s="38"/>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B219" s="41"/>
-      <c r="C219" s="41"/>
+      <c r="B219" s="38"/>
+      <c r="C219" s="38"/>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B220" s="41"/>
-      <c r="C220" s="41"/>
+      <c r="B220" s="38"/>
+      <c r="C220" s="38"/>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B221" s="41"/>
-      <c r="C221" s="41"/>
+      <c r="B221" s="38"/>
+      <c r="C221" s="38"/>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B222" s="41"/>
-      <c r="C222" s="41"/>
+      <c r="B222" s="38"/>
+      <c r="C222" s="38"/>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B223" s="41"/>
-      <c r="C223" s="41"/>
+      <c r="B223" s="38"/>
+      <c r="C223" s="38"/>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B224" s="41"/>
-      <c r="C224" s="41"/>
+      <c r="B224" s="38"/>
+      <c r="C224" s="38"/>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B225" s="41"/>
-      <c r="C225" s="41"/>
+      <c r="B225" s="38"/>
+      <c r="C225" s="38"/>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B226" s="41"/>
-      <c r="C226" s="41"/>
+      <c r="B226" s="38"/>
+      <c r="C226" s="38"/>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="41"/>
-      <c r="C227" s="41"/>
+      <c r="B227" s="38"/>
+      <c r="C227" s="38"/>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B228" s="41"/>
-      <c r="C228" s="41"/>
+      <c r="B228" s="38"/>
+      <c r="C228" s="38"/>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" s="41"/>
-      <c r="C229" s="41"/>
+      <c r="B229" s="38"/>
+      <c r="C229" s="38"/>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B230" s="41"/>
-      <c r="C230" s="41"/>
+      <c r="B230" s="38"/>
+      <c r="C230" s="38"/>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" s="41"/>
-      <c r="C231" s="41"/>
+      <c r="B231" s="38"/>
+      <c r="C231" s="38"/>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B232" s="41"/>
-      <c r="C232" s="41"/>
+      <c r="B232" s="38"/>
+      <c r="C232" s="38"/>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B233" s="41"/>
-      <c r="C233" s="41"/>
+      <c r="B233" s="38"/>
+      <c r="C233" s="38"/>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B234" s="41"/>
-      <c r="C234" s="41"/>
+      <c r="B234" s="38"/>
+      <c r="C234" s="38"/>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B235" s="41"/>
-      <c r="C235" s="41"/>
+      <c r="B235" s="38"/>
+      <c r="C235" s="38"/>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B236" s="41"/>
-      <c r="C236" s="41"/>
+      <c r="B236" s="38"/>
+      <c r="C236" s="38"/>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B237" s="41"/>
-      <c r="C237" s="41"/>
+      <c r="B237" s="38"/>
+      <c r="C237" s="38"/>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B238" s="41"/>
-      <c r="C238" s="41"/>
+      <c r="B238" s="38"/>
+      <c r="C238" s="38"/>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B239" s="41"/>
-      <c r="C239" s="41"/>
+      <c r="B239" s="38"/>
+      <c r="C239" s="38"/>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B240" s="41"/>
-      <c r="C240" s="41"/>
+      <c r="B240" s="38"/>
+      <c r="C240" s="38"/>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B241" s="41"/>
-      <c r="C241" s="41"/>
+      <c r="B241" s="38"/>
+      <c r="C241" s="38"/>
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B242" s="41"/>
-      <c r="C242" s="41"/>
+      <c r="B242" s="38"/>
+      <c r="C242" s="38"/>
     </row>
     <row r="243" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B243" s="41"/>
-      <c r="C243" s="41"/>
+      <c r="B243" s="38"/>
+      <c r="C243" s="38"/>
     </row>
     <row r="244" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B244" s="41"/>
-      <c r="C244" s="41"/>
+      <c r="B244" s="38"/>
+      <c r="C244" s="38"/>
     </row>
     <row r="245" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B245" s="41"/>
-      <c r="C245" s="41"/>
+      <c r="B245" s="38"/>
+      <c r="C245" s="38"/>
     </row>
     <row r="246" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B246" s="41"/>
-      <c r="C246" s="41"/>
+      <c r="B246" s="38"/>
+      <c r="C246" s="38"/>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B247" s="41"/>
-      <c r="C247" s="41"/>
+      <c r="B247" s="38"/>
+      <c r="C247" s="38"/>
     </row>
     <row r="248" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B248" s="41"/>
-      <c r="C248" s="41"/>
+      <c r="B248" s="38"/>
+      <c r="C248" s="38"/>
     </row>
     <row r="249" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B249" s="41"/>
-      <c r="C249" s="41"/>
+      <c r="B249" s="38"/>
+      <c r="C249" s="38"/>
     </row>
     <row r="250" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B250" s="41"/>
-      <c r="C250" s="41"/>
+      <c r="B250" s="38"/>
+      <c r="C250" s="38"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -2400,13 +2436,38 @@
     <protectedRange sqref="B19:B20" name="Rango1_5_1_1"/>
     <protectedRange sqref="C19:C20" name="Rango1_6_1_1"/>
   </protectedRanges>
-  <mergeCells count="51">
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H38"/>
+  <mergeCells count="50">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G24:H24"/>
@@ -2419,39 +2480,13 @@
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H38"/>
+    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>